<commit_message>
removed blank line from people data
</commit_message>
<xml_diff>
--- a/data/mn_county_estimates_sdc_2019_tcm36-442553.xlsx
+++ b/data/mn_county_estimates_sdc_2019_tcm36-442553.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mnscu-my.sharepoint.com/personal/vp9570vg_go_minnstate_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41756102466679fd/Documents/Carpenter-Gardin-Knoll-2022-EDA-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91C734B1-A85B-4762-847C-575A6A3EA25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{91C734B1-A85B-4762-847C-575A6A3EA25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C47DC4C-9598-4511-9E3B-077F0FCE8F3D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COUNTY_ESTIMATES_2019" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t>County Code</t>
   </si>
@@ -580,9 +580,6 @@
   </si>
   <si>
     <t>Yellow Medicine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <r>
@@ -643,7 +640,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,13 +699,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1048,16 +1044,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C63" sqref="C63"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C83" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
@@ -1068,7 +1064,7 @@
     <col min="7" max="7" width="34.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +1087,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1110,7 @@
         <v>2.0972334139135098</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1137,7 +1133,7 @@
         <v>2.7127157013174501</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1160,7 +1156,7 @@
         <v>2.3939287471014001</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1179,7 @@
         <v>2.48701298701299</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1206,7 +1202,7 @@
         <v>2.4266138855054802</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1225,7 @@
         <v>2.1707644166294102</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1252,7 +1248,7 @@
         <v>2.3801677319244798</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1275,7 +1271,7 @@
         <v>2.1965983906364301</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1298,7 +1294,7 @@
         <v>2.4526338608280902</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1321,7 +1317,7 @@
         <v>2.7658450245971999</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1344,7 +1340,7 @@
         <v>2.3318866882348299</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1367,7 +1363,7 @@
         <v>2.2588555858310602</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1390,7 +1386,7 @@
         <v>2.6502848315149201</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1413,7 +1409,7 @@
         <v>2.4376185958254299</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1436,7 +1432,7 @@
         <v>2.4065782200110601</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1459,7 +1455,7 @@
         <v>1.99963058736609</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1482,7 +1478,7 @@
         <v>2.2797755144460599</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1505,7 +1501,7 @@
         <v>2.3423652477117498</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1528,7 +1524,7 @@
         <v>2.5880036789679699</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1551,7 +1547,7 @@
         <v>2.6308198380566798</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1574,7 +1570,7 @@
         <v>2.25501106922755</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1597,7 +1593,7 @@
         <v>2.17605863192182</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1620,7 +1616,7 @@
         <v>2.3712060474172501</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1643,7 +1639,7 @@
         <v>2.2695977406304899</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -1666,7 +1662,7 @@
         <v>2.3497008458840498</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -1689,7 +1685,7 @@
         <v>2.21950301204819</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1712,7 +1708,7 @@
         <v>2.38353324279394</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -1735,7 +1731,7 @@
         <v>2.28280064668574</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -1758,7 +1754,7 @@
         <v>2.3224787627967798</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -1781,7 +1777,7 @@
         <v>2.6387427669647598</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -1804,7 +1800,7 @@
         <v>2.2771562612775198</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1827,7 +1823,7 @@
         <v>2.2157798999545202</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -1850,7 +1846,7 @@
         <v>2.4764034546576199</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -1873,7 +1869,7 @@
         <v>2.4500552036725001</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -1896,7 +1892,7 @@
         <v>2.1699481865285</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1919,7 +1915,7 @@
         <v>2.1103986135181998</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -1942,7 +1938,7 @@
         <v>2.1369636963696399</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -1965,7 +1961,7 @@
         <v>2.1252805549887799</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -1988,7 +1984,7 @@
         <v>2.1630057803468201</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2011,7 +2007,7 @@
         <v>2.5389869599928998</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -2034,7 +2030,7 @@
         <v>2.1881699086939301</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -2057,7 +2053,7 @@
         <v>2.3919884169884198</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -2080,7 +2076,7 @@
         <v>2.39334862385321</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -2103,7 +2099,7 @@
         <v>2.7114427860696502</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -2126,7 +2122,7 @@
         <v>2.3286432160803998</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -2149,7 +2145,7 @@
         <v>2.19441934026209</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -2172,7 +2168,7 @@
         <v>2.45677820677821</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>101</v>
       </c>
@@ -2195,7 +2191,7 @@
         <v>2.4788217173661899</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -2218,7 +2214,7 @@
         <v>2.4523329600597199</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -2241,7 +2237,7 @@
         <v>2.46572089244422</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>107</v>
       </c>
@@ -2264,7 +2260,7 @@
         <v>2.20882433543437</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -2287,7 +2283,7 @@
         <v>2.4153869778869801</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -2310,7 +2306,7 @@
         <v>2.6597633136094698</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -2333,7 +2329,7 @@
         <v>2.2876962395034699</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -2356,7 +2352,7 @@
         <v>2.4519080181730799</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -2379,7 +2375,7 @@
         <v>2.3171104496822501</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -2402,7 +2398,7 @@
         <v>2.27154893065457</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>121</v>
       </c>
@@ -2425,7 +2421,7 @@
         <v>2.4124147457480798</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>123</v>
       </c>
@@ -2448,7 +2444,7 @@
         <v>2.2298850574712601</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>125</v>
       </c>
@@ -2471,7 +2467,7 @@
         <v>2.3531330072210599</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>127</v>
       </c>
@@ -2494,7 +2490,7 @@
         <v>2.22571486513892</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>129</v>
       </c>
@@ -2517,7 +2513,7 @@
         <v>2.4956243595779402</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>131</v>
       </c>
@@ -2540,7 +2536,7 @@
         <v>2.3025787965615998</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>133</v>
       </c>
@@ -2563,7 +2559,7 @@
         <v>2.3099688473520299</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>135</v>
       </c>
@@ -2586,7 +2582,7 @@
         <v>2.2703047710228201</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>137</v>
       </c>
@@ -2609,7 +2605,7 @@
         <v>2.51157788181703</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>139</v>
       </c>
@@ -2632,7 +2628,7 @@
         <v>2.3348729792147802</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>141</v>
       </c>
@@ -2655,7 +2651,7 @@
         <v>2.4092874299439599</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -2678,7 +2674,7 @@
         <v>2.2084471187225199</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>145</v>
       </c>
@@ -2701,7 +2697,7 @@
         <v>2.90066264347415</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -2724,7 +2720,7 @@
         <v>2.8667289381704202</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -2747,7 +2743,7 @@
         <v>2.4456485495165099</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>151</v>
       </c>
@@ -2770,7 +2766,7 @@
         <v>2.5332332018419801</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -2793,7 +2789,7 @@
         <v>2.4848875908442598</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>155</v>
       </c>
@@ -2816,7 +2812,7 @@
         <v>2.36300454423951</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -2839,7 +2835,7 @@
         <v>2.20787325972156</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>159</v>
       </c>
@@ -2862,7 +2858,7 @@
         <v>2.44596360711772</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>161</v>
       </c>
@@ -2885,7 +2881,7 @@
         <v>2.1429539295393001</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>163</v>
       </c>
@@ -2908,7 +2904,7 @@
         <v>2.3800089047194999</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>165</v>
       </c>
@@ -2931,7 +2927,7 @@
         <v>2.28692201518288</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>167</v>
       </c>
@@ -2954,7 +2950,7 @@
         <v>2.4137695978186802</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>169</v>
       </c>
@@ -2977,7 +2973,7 @@
         <v>2.6388396766245101</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>171</v>
       </c>
@@ -3000,7 +2996,7 @@
         <v>2.3975072334742902</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>173</v>
       </c>
@@ -3023,7 +3019,7 @@
         <v>2.2388499815702199</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -3046,7 +3042,7 @@
         <v>2.3526318425401902</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>177</v>
       </c>
@@ -3069,7 +3065,7 @@
         <v>2.7967385329505898</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>179</v>
       </c>
@@ -3090,20 +3086,6 @@
       </c>
       <c r="G88" s="1">
         <v>2.2825350749879099</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="C89" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3121,59 +3103,59 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3183,21 +3165,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E42F6C70DA1BC4F965DA9EB3D478A8D" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1a4a6d5ab281bf17fb93c996464fa5ec">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="01ffc0cf-b960-463a-98dd-659dec84612b" xmlns:ns4="a579f9ac-899d-4f67-98c5-445d06cfd828" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d4c8c88054ee13708285781856cd68a" ns3:_="" ns4:_="">
     <xsd:import namespace="01ffc0cf-b960-463a-98dd-659dec84612b"/>
@@ -3382,14 +3349,53 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201EFD9D-626B-4BB2-B443-7977F1B8540A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5E92199-8DEE-4C38-BBFB-55B2A000FDD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="01ffc0cf-b960-463a-98dd-659dec84612b"/>
+    <ds:schemaRef ds:uri="a579f9ac-899d-4f67-98c5-445d06cfd828"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5ACDE1F-F9A9-46C1-A735-2C2212D18FB2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5ACDE1F-F9A9-46C1-A735-2C2212D18FB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5E92199-8DEE-4C38-BBFB-55B2A000FDD6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201EFD9D-626B-4BB2-B443-7977F1B8540A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>